<commit_message>
2025-07-08 Added Kanji Images for n3
</commit_message>
<xml_diff>
--- a/public/docs/kanji_n3.xlsx
+++ b/public/docs/kanji_n3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Kanji</t>
   </si>
@@ -30,94 +30,145 @@
     <t>English</t>
   </si>
   <si>
+    <t>かん</t>
+  </si>
+  <si>
+    <t>そう</t>
+  </si>
+  <si>
+    <t>あい</t>
+  </si>
+  <si>
+    <t>き</t>
+  </si>
+  <si>
+    <t>けい</t>
+  </si>
+  <si>
+    <t>さい</t>
+  </si>
+  <si>
+    <t>じょう</t>
+  </si>
+  <si>
+    <t>ほう</t>
+  </si>
+  <si>
+    <t>せつ</t>
+  </si>
+  <si>
+    <t>feeling</t>
+  </si>
+  <si>
+    <t>thought</t>
+  </si>
+  <si>
+    <t>love</t>
+  </si>
+  <si>
+    <t>machine</t>
+  </si>
+  <si>
+    <t>finish / settle</t>
+  </si>
+  <si>
+    <t>emotion</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>establish</t>
+  </si>
+  <si>
+    <t>pipe / manage</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>感</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_feeling.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>想</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_thought.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>愛</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_love.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>機</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_machine.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>経</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>pass through / manage</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_pass_through.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>済</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_finish.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>情</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_emotion.webp</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>報</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_report.png</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>設</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_establish.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>管</t>
-  </si>
-  <si>
-    <t>かん</t>
-  </si>
-  <si>
-    <t>そう</t>
-  </si>
-  <si>
-    <t>あい</t>
-  </si>
-  <si>
-    <t>き</t>
-  </si>
-  <si>
-    <t>けい</t>
-  </si>
-  <si>
-    <t>さい</t>
-  </si>
-  <si>
-    <t>じょう</t>
-  </si>
-  <si>
-    <t>ほう</t>
-  </si>
-  <si>
-    <t>せつ</t>
-  </si>
-  <si>
-    <t>feeling</t>
-  </si>
-  <si>
-    <t>thought</t>
-  </si>
-  <si>
-    <t>love</t>
-  </si>
-  <si>
-    <t>machine</t>
-  </si>
-  <si>
-    <t>pass through / manage</t>
-  </si>
-  <si>
-    <t>finish / settle</t>
-  </si>
-  <si>
-    <t>emotion</t>
-  </si>
-  <si>
-    <t>report</t>
-  </si>
-  <si>
-    <t>establish</t>
-  </si>
-  <si>
-    <t>pipe / manage</t>
-  </si>
-  <si>
-    <t>ImageName</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n3_manage.png</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -496,7 +547,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -512,121 +563,152 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>